<commit_message>
updated and added templates
</commit_message>
<xml_diff>
--- a/ISRaD_data_files/Hapsari_2019.xlsx
+++ b/ISRaD_data_files/Hapsari_2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f0076db\Documents\GitHub\ISRaD\ISRaD_data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{12019E13-C35B-4074-BBAA-17EE30A1A088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{347A52FA-C30A-45BC-9B3D-5395ADFC67F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21840" tabRatio="645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="645" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1435" uniqueCount="1004">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1435" uniqueCount="1003">
   <si>
     <t>curator_name</t>
   </si>
@@ -4113,9 +4113,6 @@
   </si>
   <si>
     <t>SA-2-102</t>
-  </si>
-  <si>
-    <t>bulk</t>
   </si>
   <si>
     <t>Plant_material</t>
@@ -6291,8 +6288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q985"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.08984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -8830,8 +8827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AZ1502"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView showZeros="0" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AD15" sqref="AD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.08984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -14528,8 +14525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AS63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17794,8 +17791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:DJ987"/>
   <sheetViews>
-    <sheetView topLeftCell="AN1" workbookViewId="0">
-      <selection activeCell="BK15" sqref="BK15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="BK14" sqref="BK14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.08984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -19259,7 +19256,8 @@
       <c r="BJ6" s="5">
         <v>0.95320308252947539</v>
       </c>
-      <c r="BK6" s="5">
+      <c r="BK6" s="5"/>
+      <c r="BL6" s="5">
         <v>2.37321818132572E-4</v>
       </c>
       <c r="BM6" s="5"/>
@@ -21046,7 +21044,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AG63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -21710,8 +21708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:BZ1002"/>
   <sheetViews>
-    <sheetView topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AL5" sqref="AL5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.08984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -22455,10 +22453,10 @@
         <v>228</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>964</v>
@@ -22500,14 +22498,13 @@
       <c r="AE4" s="5"/>
       <c r="AF4" s="5"/>
       <c r="AG4" s="5"/>
-      <c r="AI4" s="5"/>
       <c r="AK4" s="5">
         <v>1.0049999999999999</v>
       </c>
-      <c r="AL4" s="5">
+      <c r="AL4" s="5"/>
+      <c r="AM4" s="5">
         <v>1E-4</v>
       </c>
-      <c r="AM4" s="5"/>
       <c r="AN4" s="5"/>
       <c r="AO4" s="5"/>
       <c r="AP4" s="5"/>
@@ -22546,10 +22543,10 @@
         <v>437</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>964</v>
@@ -22597,7 +22594,8 @@
       <c r="AK5" s="5">
         <v>0.98615425908502641</v>
       </c>
-      <c r="AL5" s="5">
+      <c r="AL5" s="5"/>
+      <c r="AM5" s="5">
         <v>1.2276288548301089E-4</v>
       </c>
       <c r="AN5" s="5"/>

</xml_diff>